<commit_message>
update Self Assessment Form
</commit_message>
<xml_diff>
--- a/Self Assessment Form.xlsx
+++ b/Self Assessment Form.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fabio/Documents/Teaching/COM3504-6504 Intelligent Web/Assignment/2021-2022/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kate/WebstormProjects/assignments-/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{261A505A-0F04-B644-A87E-F096492F9398}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC4E8970-629F-E04D-B78A-E3A45F0A1BA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="220" yWindow="500" windowWidth="38180" windowHeight="19940" xr2:uid="{9384817B-0988-A24F-9D66-74DAD74AC274}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{9384817B-0988-A24F-9D66-74DAD74AC274}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,9 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -34,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="67">
   <si>
     <t>Team Name</t>
   </si>
@@ -67,9 +65,6 @@
   </si>
   <si>
     <t xml:space="preserve">Code Organization (e.g. use of Javascript classes and modules, distribution of directories etc).  </t>
-  </si>
-  <si>
-    <t>instructions</t>
   </si>
   <si>
     <t>Web App</t>
@@ -213,45 +208,69 @@
     <t>Github repo URL</t>
   </si>
   <si>
+    <t>it impements the document selection correctly</t>
+  </si>
+  <si>
+    <t>it impements the chat function correctly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It uses IndexedDB correctly </t>
+  </si>
+  <si>
+    <t>It stores the documents correctly</t>
+  </si>
+  <si>
+    <t>Correct use of Axios</t>
+  </si>
+  <si>
+    <t>Have you followed the required work allocation?</t>
+  </si>
+  <si>
+    <t>If no, why?</t>
+  </si>
+  <si>
+    <t>Insert your evaluation of the quality of your solution in the drop down cells (0 - not implemented, 1- low quality, 2 - fair, 3 good, 4 - excellent)</t>
+  </si>
+  <si>
+    <t>Mengyao Piao</t>
+    <phoneticPr fontId="23" type="noConversion"/>
+  </si>
+  <si>
+    <t>Chaoda Song</t>
+    <phoneticPr fontId="23" type="noConversion"/>
+  </si>
+  <si>
+    <t>Jun Liu</t>
+    <phoneticPr fontId="23" type="noConversion"/>
+  </si>
+  <si>
+    <t>please do not modify the form; do not introduce new columns; do not introduce new rows; we will process the form automatically!!</t>
+    <phoneticPr fontId="23" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://github.com/upc2017/assignments-</t>
+  </si>
+  <si>
     <t>Hav you given access to the lecturer and lab assistants?</t>
-  </si>
-  <si>
-    <t>it impements the document selection correctly</t>
-  </si>
-  <si>
-    <t>it impements the chat function correctly</t>
-  </si>
-  <si>
-    <t xml:space="preserve">It uses IndexedDB correctly </t>
-  </si>
-  <si>
-    <t>It stores the documents correctly</t>
-  </si>
-  <si>
-    <t>Correct use of Axios</t>
-  </si>
-  <si>
-    <t>Have you followed the required work allocation?</t>
-  </si>
-  <si>
-    <t>If no, why?</t>
-  </si>
-  <si>
-    <t>please do not modify the form; do not introduce new columns; do not introduce new rows; we will process the form automatically!!</t>
-  </si>
-  <si>
-    <t>Insert your evaluation of the quality of your solution in the drop down cells (0 - not implemented, 1- low quality, 2 - fair, 3 good, 4 - excellent)</t>
+    <phoneticPr fontId="23" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>instructions</t>
+    <phoneticPr fontId="23" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="24">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -259,7 +278,7 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -384,7 +403,7 @@
       <b/>
       <sz val="18"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -394,6 +413,13 @@
       <color theme="1"/>
       <name val="Courier New"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -542,24 +568,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Default 1" xfId="1" xr:uid="{4CFB9B37-B9E9-0348-B0C6-CB853B61E7A3}"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -575,7 +601,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -873,11 +899,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A704EA58-8849-E44F-8AE0-CB0AA8314588}">
   <dimension ref="A1:E80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
+      <selection activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
   <cols>
     <col min="1" max="1" width="30.83203125" style="18" customWidth="1"/>
     <col min="2" max="2" width="45.1640625" style="30" customWidth="1"/>
@@ -886,73 +912,84 @@
     <col min="5" max="5" width="139.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="38" customFormat="1" ht="95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="40" t="s">
-        <v>60</v>
-      </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-    </row>
-    <row r="2" spans="1:5" s="38" customFormat="1" ht="95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="38" customFormat="1" ht="95" customHeight="1">
+      <c r="A1" s="44" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+    </row>
+    <row r="2" spans="1:5" s="38" customFormat="1" ht="95" customHeight="1">
       <c r="A2" s="37"/>
       <c r="B2" s="39"/>
       <c r="C2" s="39"/>
       <c r="D2" s="39"/>
     </row>
-    <row r="3" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="18">
       <c r="A3" s="14" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="24"/>
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="18">
       <c r="A4" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="25"/>
+      <c r="B4" s="25" t="s">
+        <v>59</v>
+      </c>
       <c r="C4" s="2"/>
     </row>
-    <row r="5" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="18">
       <c r="A5" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="25"/>
+      <c r="B5" s="25" t="s">
+        <v>60</v>
+      </c>
       <c r="C5" s="2"/>
     </row>
-    <row r="6" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="18">
       <c r="A6" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="25"/>
+      <c r="B6" s="25" t="s">
+        <v>61</v>
+      </c>
       <c r="C6" s="2"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" s="16"/>
       <c r="B7" s="26"/>
       <c r="C7" s="4"/>
     </row>
-    <row r="8" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="19">
       <c r="A8" s="6"/>
       <c r="B8" s="27"/>
       <c r="C8" s="7"/>
     </row>
-    <row r="9" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="19">
       <c r="A9" s="6"/>
       <c r="B9" s="27"/>
       <c r="C9" s="7"/>
     </row>
-    <row r="10" spans="1:5" ht="36" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="36">
       <c r="A10" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="B10" s="24"/>
-      <c r="C10" s="45" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" s="11" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="B10" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="C10" s="43" t="s">
+        <v>64</v>
+      </c>
+      <c r="D10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" s="11" customFormat="1" ht="120">
       <c r="A11" s="6" t="s">
         <v>4</v>
       </c>
@@ -960,402 +997,402 @@
         <v>5</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>11</v>
+        <v>66</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E11" s="10" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" s="13" customFormat="1">
       <c r="A12" s="17" t="s">
         <v>7</v>
       </c>
       <c r="B12" s="28"/>
     </row>
-    <row r="13" spans="1:5" ht="108" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="108">
       <c r="B13" s="29" t="s">
         <v>8</v>
       </c>
       <c r="D13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="36" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="36">
       <c r="B14" s="24" t="s">
         <v>9</v>
       </c>
       <c r="D14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="54" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="54">
       <c r="B15" s="24" t="s">
         <v>10</v>
       </c>
       <c r="D15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
       <c r="A19" s="18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="54">
+      <c r="B20" s="36" t="s">
+        <v>46</v>
+      </c>
+      <c r="D20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="36">
+      <c r="B21" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="D21">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="36">
+      <c r="B22" s="30" t="s">
+        <v>52</v>
+      </c>
+      <c r="D22">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="36">
+      <c r="B23" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="D23">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="54">
+      <c r="B24" s="26" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" ht="54" x14ac:dyDescent="0.25">
-      <c r="B20" s="36" t="s">
-        <v>47</v>
-      </c>
-      <c r="D20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="36" x14ac:dyDescent="0.25">
-      <c r="B21" s="30" t="s">
+      <c r="D24">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="18">
+      <c r="B25" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="D25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="90">
+      <c r="B26" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="D26">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="18">
+      <c r="B27" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="D21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="36" x14ac:dyDescent="0.25">
-      <c r="B22" s="30" t="s">
-        <v>54</v>
-      </c>
-      <c r="D22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="36" x14ac:dyDescent="0.25">
-      <c r="B23" s="30" t="s">
-        <v>37</v>
-      </c>
-      <c r="D23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="54" x14ac:dyDescent="0.25">
-      <c r="B24" s="26" t="s">
-        <v>13</v>
-      </c>
-      <c r="D24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="B25" s="26" t="s">
+      <c r="D27">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="36">
+      <c r="B28" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="D25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="90" x14ac:dyDescent="0.25">
-      <c r="B26" s="30" t="s">
-        <v>38</v>
-      </c>
-      <c r="D26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="B27" s="26" t="s">
-        <v>55</v>
-      </c>
-      <c r="D27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="36" x14ac:dyDescent="0.25">
-      <c r="B28" s="26" t="s">
+      <c r="D28">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="18">
+      <c r="B29" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="D28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="B29" s="26" t="s">
+      <c r="D29">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="18">
+      <c r="B30" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="D29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="B30" s="26" t="s">
+      <c r="D30">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="306">
+      <c r="B31" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="C31" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="324" x14ac:dyDescent="0.25">
-      <c r="B31" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="C31" s="4" t="s">
+      <c r="D31" s="5"/>
+    </row>
+    <row r="33" spans="1:4" ht="18">
+      <c r="A33" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="D31" s="5"/>
-    </row>
-    <row r="33" spans="1:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="A33" s="18" t="s">
+      <c r="B33" s="32" t="s">
         <v>19</v>
-      </c>
-      <c r="B33" s="32" t="s">
-        <v>20</v>
       </c>
       <c r="C33" s="4"/>
       <c r="D33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="36" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="36">
       <c r="B34" s="32" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C34" s="4"/>
       <c r="D34">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="36" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="18">
       <c r="B35" s="32" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C35" s="4"/>
       <c r="D35">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="18">
       <c r="B36" s="32" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C36" s="4"/>
       <c r="D36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="72" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="72">
       <c r="B37" s="32" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C37" s="4"/>
       <c r="D37">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="36" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="36">
       <c r="B38" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C38" s="4"/>
       <c r="D38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="36" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="18">
       <c r="B39" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C39" s="12"/>
       <c r="D39">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="18">
       <c r="B40" s="31" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C40" s="4"/>
       <c r="D40">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="18">
       <c r="B41" s="31" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C41" s="4"/>
       <c r="D41">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="162" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="162">
       <c r="B42" s="31" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C42" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" s="18" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="18" t="s">
+      <c r="B46" s="23" t="s">
         <v>24</v>
-      </c>
-      <c r="B46" s="23" t="s">
-        <v>25</v>
       </c>
       <c r="C46" s="12"/>
       <c r="D46">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" ht="49" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="49">
       <c r="B47" s="23" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C47" s="12"/>
       <c r="D47">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
       <c r="B48" s="23" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C48" s="12"/>
       <c r="D48">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="18">
       <c r="B49" s="33" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C49" s="21"/>
       <c r="D49">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="18">
       <c r="B50" s="33" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C50" s="21"/>
       <c r="D50">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" ht="288" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="288">
       <c r="B51" s="31" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C51" s="21" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
       <c r="A53" s="18" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="18">
       <c r="B54" s="30" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D54">
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" ht="18">
       <c r="B55" s="30" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D55">
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" ht="90">
       <c r="B56" s="31" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C56" s="21" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
       <c r="A58" s="18" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="72">
+      <c r="B59" s="30" t="s">
         <v>39</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" ht="72" x14ac:dyDescent="0.25">
-      <c r="B59" s="30" t="s">
-        <v>40</v>
       </c>
       <c r="D59">
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4">
       <c r="A61" s="18" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" ht="54">
+      <c r="B62" s="30" t="s">
         <v>29</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" ht="54" x14ac:dyDescent="0.25">
-      <c r="B62" s="30" t="s">
-        <v>30</v>
       </c>
       <c r="D62">
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="54" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" ht="54">
       <c r="B63" s="30" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D63">
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:4" ht="54" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" ht="54">
       <c r="B64" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="C64" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="C64" s="21" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="66" spans="1:4">
       <c r="A66" s="19" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" ht="54" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" ht="54">
       <c r="A67" s="20"/>
       <c r="B67" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="C67" t="s">
         <v>49</v>
       </c>
-      <c r="C67" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="68" spans="1:4">
       <c r="A68" s="34" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" s="42" customFormat="1" ht="32" x14ac:dyDescent="0.2">
-      <c r="A69" s="43" t="s">
-        <v>58</v>
-      </c>
-      <c r="B69" s="44"/>
-      <c r="C69" s="44" t="s">
-        <v>59</v>
-      </c>
-      <c r="D69" s="44"/>
-    </row>
-    <row r="70" spans="1:4" s="42" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A70" s="43"/>
-      <c r="B70" s="44"/>
-      <c r="C70" s="44"/>
-      <c r="D70" s="44"/>
-    </row>
-    <row r="71" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" s="40" customFormat="1" ht="32">
+      <c r="A69" s="41" t="s">
+        <v>56</v>
+      </c>
+      <c r="B69" s="42"/>
+      <c r="C69" s="42" t="s">
+        <v>57</v>
+      </c>
+      <c r="D69" s="42"/>
+    </row>
+    <row r="70" spans="1:4" s="40" customFormat="1" ht="16">
+      <c r="A70" s="41"/>
+      <c r="B70" s="42"/>
+      <c r="C70" s="42"/>
+      <c r="D70" s="42"/>
+    </row>
+    <row r="71" spans="1:4" ht="16">
       <c r="B71" s="34" t="s">
         <v>1</v>
       </c>
@@ -1366,47 +1403,48 @@
         <v>3</v>
       </c>
     </row>
-    <row r="72" spans="1:4" ht="49" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" ht="49">
       <c r="A72" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B72" s="4"/>
       <c r="C72" s="4"/>
       <c r="D72" s="5"/>
     </row>
-    <row r="73" spans="1:4" ht="81" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" ht="81">
       <c r="A73" s="35" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B73" s="4"/>
       <c r="C73" s="4"/>
       <c r="D73" s="5"/>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4">
       <c r="A74" s="20"/>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4">
       <c r="A75" s="20"/>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4">
       <c r="A76" s="19"/>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4">
       <c r="A77" s="20"/>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4">
       <c r="A78" s="19"/>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4">
       <c r="A79" s="20"/>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4">
       <c r="A80" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:D1"/>
   </mergeCells>
+  <phoneticPr fontId="23" type="noConversion"/>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D10" xr:uid="{E6C66EE8-0A25-D749-854A-FC5B1F6D2E99}">
       <formula1>"No, Yes"</formula1>

</xml_diff>